<commit_message>
Be: Update branches_accounts.xlsx & fix email/phone_no login
</commit_message>
<xml_diff>
--- a/public/be-export/branches_accounts.xlsx
+++ b/public/be-export/branches_accounts.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Wife\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Truong Khanh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1263F30A-3096-4673-8873-AB3E4D628E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB46F7A9-8C70-471A-9E34-B08BAC15A439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28910" yWindow="1630" windowWidth="29020" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="branch_full_name">Sheet1!#REF!</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
   <si>
     <t>branch</t>
   </si>
@@ -124,9 +140,6 @@
     <t>caphemuoichulong.71hg@gmail.com</t>
   </si>
   <si>
-    <t>O939640008</t>
-  </si>
-  <si>
     <t>caphemuoichulong.187llq@gmail.com</t>
   </si>
   <si>
@@ -196,9 +209,6 @@
     <t>82f83c4f</t>
   </si>
   <si>
-    <t>Chulong71hg</t>
-  </si>
-  <si>
     <t>Caphemuoi129tktq</t>
   </si>
   <si>
@@ -211,18 +221,12 @@
     <t>194CMT8</t>
   </si>
   <si>
-    <t>307DNC</t>
-  </si>
-  <si>
     <t>Cfm161ntt</t>
   </si>
   <si>
     <t>d781fbe6</t>
   </si>
   <si>
-    <t>88888888</t>
-  </si>
-  <si>
     <t>4c59a80b</t>
   </si>
   <si>
@@ -257,6 +261,27 @@
   </si>
   <si>
     <t>Caphemuoi@544td</t>
+  </si>
+  <si>
+    <t>caphemuoichulong.dl@gmail.com</t>
+  </si>
+  <si>
+    <t>b6ce7540</t>
+  </si>
+  <si>
+    <t>caphemuoithanhthai@gmail.com</t>
+  </si>
+  <si>
+    <t>Đường Láng</t>
+  </si>
+  <si>
+    <t>Lê Văn Việt</t>
+  </si>
+  <si>
+    <t>Thành Thái</t>
+  </si>
+  <si>
+    <t>0939640008</t>
   </si>
 </sst>
 </file>
@@ -315,12 +340,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -640,13 +672,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -655,83 +687,83 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="D2" s="2">
-        <v>83060</v>
+        <v>81864</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="D3" s="2">
-        <v>82940</v>
+        <v>82946</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="D4" s="2">
-        <v>83060</v>
+        <v>82946</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4">
+        <v>88888888</v>
       </c>
       <c r="D5" s="2">
-        <v>82947</v>
+        <v>83060</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="D6" s="2">
-        <v>83060</v>
+        <v>81864</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="D7" s="2">
         <v>83060</v>
@@ -739,69 +771,69 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="D8" s="2">
-        <v>83060</v>
+        <v>81864</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>61</v>
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="D9" s="2">
-        <v>83060</v>
+        <v>81864</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="D10" s="2">
-        <v>83060</v>
+        <v>81864</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>63</v>
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D11" s="2">
-        <v>83060</v>
+        <v>81864</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>64</v>
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="4">
+        <v>123123</v>
       </c>
       <c r="D12" s="2">
         <v>83060</v>
@@ -809,27 +841,27 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="D13" s="2">
-        <v>82946</v>
+        <v>83060</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>66</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="D14" s="2">
         <v>83060</v>
@@ -837,13 +869,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>67</v>
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="D15" s="2">
         <v>83060</v>
@@ -851,41 +883,41 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>68</v>
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="D16" s="2">
-        <v>81864</v>
+        <v>82940</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>69</v>
+        <v>21</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="D17" s="2">
-        <v>83060</v>
+        <v>81864</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>4</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="D18" s="2">
         <v>83060</v>
@@ -893,55 +925,55 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>71</v>
+        <v>11</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="D19" s="2">
-        <v>81864</v>
+        <v>83060</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>72</v>
+        <v>8</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="4">
+        <v>123123</v>
       </c>
       <c r="D20" s="2">
-        <v>81864</v>
+        <v>83060</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D21" s="2">
-        <v>81864</v>
+        <v>82947</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>22</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="D22" s="2">
         <v>81864</v>
@@ -949,61 +981,109 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>75</v>
+        <v>20</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="D23" s="2">
-        <v>81864</v>
+        <v>83060</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>76</v>
+        <v>19</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="D24" s="2">
-        <v>81864</v>
+        <v>83060</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="D25" s="2">
-        <v>81864</v>
+        <v>83060</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>78</v>
+        <v>24</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D26" s="2">
         <v>81864</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="2">
+        <v>81864</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="2">
+        <v>82941</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="2">
+        <v>82941</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{83C38CD9-BEC8-4813-80C4-F0A6927A280E}">
+      <formula1>branch_full_name</formula1>
+    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A3:A29" xr:uid="{3BCBA7DE-D682-4DC2-972A-3D4E301C41DB}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Be: Fix login data type, update branches_account
</commit_message>
<xml_diff>
--- a/public/be-export/branches_accounts.xlsx
+++ b/public/be-export/branches_accounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Truong Khanh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB46F7A9-8C70-471A-9E34-B08BAC15A439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE605C0B-4F28-4754-B0D7-76C6E5155D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28910" yWindow="1630" windowWidth="29020" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Nguyễn Huệ</t>
   </si>
   <si>
-    <t>3.26 Quang Trung</t>
-  </si>
-  <si>
     <t>Cộng Hòa</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>CMT8</t>
   </si>
   <si>
-    <t>Tân Hòa Đông</t>
-  </si>
-  <si>
     <t>161 Ngô Tất Tố</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>17A Ngô Tất Tố</t>
   </si>
   <si>
-    <t>Công Trường Dân Chủ</t>
-  </si>
-  <si>
     <t>Nguyễn Hữu Cảnh</t>
   </si>
   <si>
@@ -282,6 +273,15 @@
   </si>
   <si>
     <t>0939640008</t>
+  </si>
+  <si>
+    <t>Đặng Nguyên Cẩn</t>
+  </si>
+  <si>
+    <t>3/26 Quang Trung</t>
+  </si>
+  <si>
+    <t>Công Trường Quốc Tế</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -687,13 +687,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2">
         <v>81864</v>
@@ -701,13 +701,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2">
         <v>82946</v>
@@ -715,13 +715,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2">
         <v>82946</v>
@@ -729,10 +729,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4">
         <v>88888888</v>
@@ -743,13 +743,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2">
         <v>81864</v>
@@ -757,13 +757,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2">
         <v>83060</v>
@@ -771,13 +771,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2">
         <v>81864</v>
@@ -785,13 +785,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D9" s="2">
         <v>81864</v>
@@ -799,13 +799,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D10" s="2">
         <v>81864</v>
@@ -813,13 +813,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D11" s="2">
         <v>81864</v>
@@ -827,10 +827,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4">
         <v>123123</v>
@@ -841,13 +841,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="2">
         <v>83060</v>
@@ -855,13 +855,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2">
         <v>83060</v>
@@ -869,13 +869,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D15" s="2">
         <v>83060</v>
@@ -883,13 +883,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D16" s="2">
         <v>82940</v>
@@ -897,13 +897,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D17" s="2">
         <v>81864</v>
@@ -914,10 +914,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D18" s="2">
         <v>83060</v>
@@ -925,13 +925,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2">
         <v>83060</v>
@@ -939,10 +939,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4">
         <v>123123</v>
@@ -953,13 +953,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D21" s="2">
         <v>82947</v>
@@ -967,13 +967,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D22" s="2">
         <v>81864</v>
@@ -981,13 +981,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D23" s="2">
         <v>83060</v>
@@ -995,13 +995,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2">
         <v>83060</v>
@@ -1009,13 +1009,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D25" s="2">
         <v>83060</v>
@@ -1023,13 +1023,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D26" s="2">
         <v>81864</v>
@@ -1037,13 +1037,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D27" s="2">
         <v>81864</v>
@@ -1051,13 +1051,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D28" s="2">
         <v>82941</v>
@@ -1065,13 +1065,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D29" s="2">
         <v>82941</v>

</xml_diff>